<commit_message>
Update notifications and shops
</commit_message>
<xml_diff>
--- a/data/pricelists/citilink_pricelist.xlsx
+++ b/data/pricelists/citilink_pricelist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vladi\GolandProjects\StartupPCConfigurator\data\pricelists\processed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDCC9329-39C0-4AC4-ABAE-3AC98F5A9C19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A473407E-3304-48BE-9473-412E61CB9641}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4600" yWindow="3890" windowWidth="19200" windowHeight="10510" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1900" yWindow="1900" windowWidth="19200" windowHeight="10510" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -46,9 +46,6 @@
     <t>В наличии</t>
   </si>
   <si>
-    <t>https://www.dns-shop.ru/product/3239ebce09e93332/processor-amd-ryzen-5-5600x-oem/</t>
-  </si>
-  <si>
     <t>https://www.dns-shop.ru/product/d3c6a3f806feed20/processor-intel-core-i5-12400-oem/</t>
   </si>
   <si>
@@ -92,6 +89,9 @@
   </si>
   <si>
     <t>https://www.dns‑shop.ru/product/ff075c9cbcc93332</t>
+  </si>
+  <si>
+    <t>https://www.citilink.ru/product/processor-amd-ryzen-5-5600x-am4-oem-100-000000065-1773829/</t>
   </si>
 </sst>
 </file>
@@ -475,7 +475,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -509,10 +509,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C2">
-        <v>14599</v>
+        <v>8990</v>
       </c>
       <c r="D2" t="s">
         <v>6</v>
@@ -521,7 +521,7 @@
         <v>7</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
@@ -529,7 +529,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C3">
         <v>17399</v>
@@ -541,7 +541,7 @@
         <v>7</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
@@ -549,7 +549,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C4">
         <v>36499</v>
@@ -561,7 +561,7 @@
         <v>7</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
@@ -569,7 +569,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5">
         <v>32499</v>
@@ -581,7 +581,7 @@
         <v>7</v>
       </c>
       <c r="F5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
@@ -589,7 +589,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C6">
         <v>46999</v>
@@ -601,7 +601,7 @@
         <v>7</v>
       </c>
       <c r="F6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
@@ -609,7 +609,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C7">
         <v>18499</v>
@@ -621,7 +621,7 @@
         <v>7</v>
       </c>
       <c r="F7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
@@ -629,7 +629,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C8">
         <v>17599</v>
@@ -641,7 +641,7 @@
         <v>7</v>
       </c>
       <c r="F8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
@@ -649,7 +649,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C9">
         <v>5399</v>
@@ -661,7 +661,7 @@
         <v>7</v>
       </c>
       <c r="F9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
@@ -669,7 +669,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C10">
         <v>11999</v>
@@ -681,7 +681,7 @@
         <v>7</v>
       </c>
       <c r="F10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
@@ -689,7 +689,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C11">
         <v>16199</v>
@@ -701,7 +701,7 @@
         <v>7</v>
       </c>
       <c r="F11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
@@ -709,7 +709,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C12">
         <v>11499</v>
@@ -721,7 +721,7 @@
         <v>7</v>
       </c>
       <c r="F12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
@@ -729,7 +729,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C13">
         <v>11999</v>
@@ -741,7 +741,7 @@
         <v>7</v>
       </c>
       <c r="F13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
@@ -749,7 +749,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C14">
         <v>5999</v>
@@ -758,10 +758,10 @@
         <v>6</v>
       </c>
       <c r="E14" t="s">
+        <v>20</v>
+      </c>
+      <c r="F14" t="s">
         <v>21</v>
-      </c>
-      <c r="F14" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
@@ -769,7 +769,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C15">
         <v>4199</v>
@@ -781,7 +781,7 @@
         <v>7</v>
       </c>
       <c r="F15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>